<commit_message>
updated w/ Nianchao's suspicious nodules
</commit_message>
<xml_diff>
--- a/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
+++ b/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Github\bmen689_group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1233B88D-298F-4992-8FD8-BE18DC6B6BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2325A27E-33A1-435C-8272-A048B75C263A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5350" yWindow="680" windowWidth="7900" windowHeight="6560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="138">
   <si>
     <t>LUNGx-CT001</t>
   </si>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:A71"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1288,7 +1288,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>26</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1607,8 +1607,11 @@
       <c r="F32" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>33</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>34</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>39</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>40</v>
       </c>
@@ -1767,8 +1770,11 @@
       <c r="F40" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -1788,7 +1794,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>43</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>44</v>
       </c>
@@ -1848,7 +1854,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -1868,7 +1874,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>47</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
added the paths as well so we can figure out which image number to use in one place rather than opening 2 files each time
</commit_message>
<xml_diff>
--- a/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
+++ b/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Github\bmen689_group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2325A27E-33A1-435C-8272-A048B75C263A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E723713C-BA96-44F6-BA97-431FC9A37AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="-12540" windowWidth="14400" windowHeight="7365" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="206">
   <si>
     <t>LUNGx-CT001</t>
   </si>
@@ -426,15 +426,6 @@
     <t xml:space="preserve">Primary lung cancer </t>
   </si>
   <si>
-    <t>looks like scarring</t>
-  </si>
-  <si>
-    <t>juxtapleural: are the center coordinates correct?</t>
-  </si>
-  <si>
-    <t>is this correct?</t>
-  </si>
-  <si>
     <t>LUNGx-CT055</t>
   </si>
   <si>
@@ -445,23 +436,229 @@
   </si>
   <si>
     <t>209, 308</t>
+  </si>
+  <si>
+    <t>LUNGx-CT001\09-24-2006-7805-CT INFUSED CHEST-62081\4-HIGH RES-69714\000218.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT002\05-25-2007-914-CT INFUSED CHEST-96111\4-HIGH RES-70218\000086.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT002\05-25-2007-914-CT INFUSED CHEST-96111\4-HIGH RES-70218\000192.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT003\03-23-2006-6667-CT NON-INFUSED CHEST-15464\5-HIGH RES-37154\000086.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT004\12-17-2006-8984-CT INFUSED CHEST-50128\5-HI-RES-19249\000110.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT004\12-17-2006-8984-CT INFUSED CHEST-50128\5-HI-RES-19249\000175.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT005\09-30-2006-18035-CT NON-INFUSED CHEST-77526\7421-HI-RES-40794\000299.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT005\09-30-2006-18035-CT NON-INFUSED CHEST-77526\7421-HI-RES-40794\000034.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT006\08-24-2006-5981-CT INFUSED CHEST-67393\4-HIGH RES-86344\000168.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT007\01-12-2007-10096-CT INFUSED CHEST-23807\6-HIGH RES-87220\000231.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT008\07-20-2006-8531-CT INFUSED CHEST-25891\6-HIGH RES-72237\000095.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT009\10-16-2006-7858-CT NON-INFUSED CHEST-42434\5-HI RES-23395\000240.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT010\01-12-2007-9020-CT INFUSED CHEST-84069\4-HIGH RES-90345\000231.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT011\09-16-2006-21584-CT INFUSED CHEST-49902\4-HIGH RES-79323\000012.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT012\04-18-2006-6242-CT INFUSED CHEST-00902\10269-HI RES-57102\000167.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT013\03-14-2007-482-CT NON-INFUSED CHEST-12952\5-HIGH RES-39835\000174.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT014\07-06-2006-20713-CT INFUSED CHEST-36309\4-HIGH RES-23604\000126.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT015\04-04-2007-7377-CT NON-INFUSED CHEST-31852\4-HIGH RES-25609\000185.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT016\03-05-2007-6934-CT INFUSED CHEST-52742\5-HI-RES-40880\000238.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT016\03-05-2007-6934-CT INFUSED CHEST-52742\5-HI-RES-40880\000014.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT017\12-27-2006-21828-80787\6-HIGH RES-38232\000268.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT017\12-27-2006-21828-80787\6-HIGH RES-38232\000125.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT018\06-16-2006-5967-CT NON-INFUSED CHEST-47430\4-HIGH RES-63542\000260.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT019\08-27-2006-17371-CT INFUSED CHEST-99144\2047-HI-RES-12730\000209.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT020\04-26-2006-7711-CT NON-INFUSED CHEST-15639\4-HIGH RES-94178\000387.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT021\01-11-2007-5614-CT INFUSED CHEST-02967\7-HIGH RES-51556\000267.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT022\06-15-2006-6501-CT INFUSED CHEST-94126\4-HIGH RES-83725\000039.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT023\07-26-2006-7322-CT INFUSED CHEST-47399\4-HIGH RES-60559\000037.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT024\07-03-2006-19062-CT INFUSED CHEST-12515\5984-HI-RES-85034\000212.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT025\03-06-2007-18111-CT INFUSED CHEST-16264\7951-HI-RES-95826\000156.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT026\06-10-2006-5920-CT INFUSED CHEST-13884\4-HIGH RES-68644\000167.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT027\01-13-2007-22246-CT INFUSED CHEST-85959\4-HIGH RES-86583\000095.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT028\04-03-2007-999-CT INFUSED CHEST-88072\4-HIGH RES-95600\000201.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT029\12-09-2006-19587-CT INFUSED CHEST-47401\6-HIGH RES-47567\000195.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT029\12-09-2006-19587-CT INFUSED CHEST-47401\6-HIGH RES-47567\000043.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT030\02-23-2006-17638-CT NON-INFUSED CHEST-29076\4217-HI-RES-52533\000160.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT031\03-18-2007-9184-CT INFUSED CHEST-25884\4-HIGH RES-45806\000192.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT032\02-18-2007-7328-CT INFUSED CHEST-36835\4-HIGH RES-33014\000126.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT033\07-08-2006-20044-CT INFUSED CHEST-73110\5-HIGH RES-73061\000072.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT034\08-18-2006-21190-CT INFUSED CHEST-26117\5-HIGH RES-98365\000242.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT035\04-18-2006-69780-CT INFUSED CHEST-95899\8-HIGH RES-38494\000197.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT035\04-18-2006-69780-CT INFUSED CHEST-95899\8-HIGH RES-38494\000016.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT036\03-01-2006-5970-B CT NON-INFUSED CHEST-61573\5-HI RES-90274\000129.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT037\02-26-2007-6066-CT INFUSED CHEST-00085\5-HIGH RES-08330\000321.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT038\03-11-2007-8134-CT INFUSED CHEST-83487\4-HIGH RES-15907\000294.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT039\08-12-2006-7552-CT INFUSED CHEST-66176\4-HIGH RES-15116\000267.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT040\08-15-2006-18203-CT INFUSED CHEST-51678\8404-HI-RES-64711\000075.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT041\06-04-2006-17420-CT NON-INFUSED CHEST-43897\2444-HI-RES-49643\000274.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT042\04-19-2006-6682-CT INFUSED CHEST-27083\4-HIGH RES-13338\000031.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT043\05-09-2007-6738-CT NON-INFUSED CHEST-98348\5-HIGH RES-56352\000008.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT043\05-09-2007-6738-CT NON-INFUSED CHEST-98348\5-HIGH RES-56352\000193.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT044\10-21-2006-19622-CT INFUSED CHEST-47108\4-HIGH RES-92720\000322.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT045\04-30-2006-7052-CT INFUSED CHEST-69003\4-HIGH RES-55992\00061.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT046\05-05-2006-20464-CT INFUSED CHEST-91911\5-HIGH RES-39013\000155.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT047\02-09-2007-6359-CT INFUSED CHEST-67102\4-HIGH RES-56113\000262.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT047\02-09-2007-6359-CT INFUSED CHEST-67102\4-HIGH RES-56113\000097.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT048\07-01-2006-18319-CT INFUSED CHEST-59897\9711-HI-RES-03740\000126.DCM</t>
+  </si>
+  <si>
+    <t>LUNGx-CT049\12-31-2006-8392-CT INFUSED CHEST-54153\4-HIGH RES-37996\000071.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT050\11-22-2006-8726-CT INFUSED CHEST-94751\6-HI-RES-69707\000242.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT051\01-13-2007-794-CT INFUSED CHEST-32081\4-HIGH RES-64483\000282.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT052\04-15-2007-9233-CT NON-INFUSED CHEST-31130\5-HIGH RES-28655\000002.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT052\04-15-2007-9233-CT NON-INFUSED CHEST-31130\5-HIGH RES-28655\000255.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT053\01-17-2007-6079-CT INFUSED CHEST-21858\4-HIGH RES-36113\000298.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT054\01-23-2007-17462-CT INFUSED CHEST-52125\4-HIGH RES-23912\000118.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT055\01-23-2007-5542-CT INFUSED CHEST-31841\6-HIGH RES-53130\000123.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT056\01-14-2007-17216-CT INFUSED CHEST-57893\4-HIGH RES-84663\000168.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT057\01-05-2007-5839-CT INFUSED CHEST-10925\4-HIGH RES-56183\0000061.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT058\01-05-2007-6746-CT NON-INFUSED CHEST-80225\5-HI-RES-93729\0000015.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT059\01-08-2007-6789-CT INFUSED CHEST-26028\5-HI RES-62275\0000034.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT059\01-08-2007-6789-CT INFUSED CHEST-26028\5-HI RES-62275\000304.dcm</t>
+  </si>
+  <si>
+    <t>LUNGx-CT060\02-20-2007-6367-CT INFUSED CHEST-13719\4-HIGH RES-42551\000035.dcm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -475,17 +672,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -497,19 +689,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -940,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -951,12 +1140,12 @@
     <col min="1" max="1" width="3.08203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="5.58203125" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3">
         <v>1</v>
       </c>
@@ -975,8 +1164,11 @@
       <c r="F1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -995,17 +1187,20 @@
       <c r="F2" t="s">
         <v>128</v>
       </c>
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
       <c r="I2">
         <v>24</v>
       </c>
       <c r="J2">
-        <v>24</v>
-      </c>
-      <c r="K2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1024,11 +1219,14 @@
       <c r="F3" t="s">
         <v>128</v>
       </c>
-      <c r="I3">
+      <c r="G3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3">
         <v>43489</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1047,8 +1245,11 @@
       <c r="F4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1067,8 +1268,11 @@
       <c r="F5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1087,8 +1291,11 @@
       <c r="F6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1107,8 +1314,11 @@
       <c r="F7" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -1127,8 +1337,11 @@
       <c r="F8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1147,8 +1360,11 @@
       <c r="F9" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -1167,8 +1383,11 @@
       <c r="F10" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -1187,8 +1406,11 @@
       <c r="F11" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -1207,8 +1429,11 @@
       <c r="F12" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -1227,8 +1452,11 @@
       <c r="F13" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -1247,8 +1475,11 @@
       <c r="F14" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -1267,8 +1498,11 @@
       <c r="F15" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1286,6 +1520,9 @@
       </c>
       <c r="F16" t="s">
         <v>128</v>
+      </c>
+      <c r="G16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1307,6 +1544,9 @@
       <c r="F17" t="s">
         <v>129</v>
       </c>
+      <c r="G17" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
@@ -1327,6 +1567,9 @@
       <c r="F18" t="s">
         <v>129</v>
       </c>
+      <c r="G18" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
@@ -1347,6 +1590,9 @@
       <c r="F19" t="s">
         <v>129</v>
       </c>
+      <c r="G19" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
@@ -1367,6 +1613,9 @@
       <c r="F20" t="s">
         <v>129</v>
       </c>
+      <c r="G20" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
@@ -1387,6 +1636,9 @@
       <c r="F21" t="s">
         <v>128</v>
       </c>
+      <c r="G21" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
@@ -1407,6 +1659,9 @@
       <c r="F22" t="s">
         <v>128</v>
       </c>
+      <c r="G22" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
@@ -1427,6 +1682,9 @@
       <c r="F23" t="s">
         <v>128</v>
       </c>
+      <c r="G23" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
@@ -1447,6 +1705,9 @@
       <c r="F24" t="s">
         <v>130</v>
       </c>
+      <c r="G24" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
@@ -1467,6 +1728,9 @@
       <c r="F25" t="s">
         <v>128</v>
       </c>
+      <c r="G25" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
@@ -1487,6 +1751,9 @@
       <c r="F26" t="s">
         <v>130</v>
       </c>
+      <c r="G26" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
@@ -1507,6 +1774,9 @@
       <c r="F27" t="s">
         <v>130</v>
       </c>
+      <c r="G27" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
@@ -1527,6 +1797,9 @@
       <c r="F28" t="s">
         <v>128</v>
       </c>
+      <c r="G28" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
@@ -1547,6 +1820,9 @@
       <c r="F29" t="s">
         <v>128</v>
       </c>
+      <c r="G29" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
@@ -1567,6 +1843,9 @@
       <c r="F30" t="s">
         <v>130</v>
       </c>
+      <c r="G30" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
@@ -1587,6 +1866,9 @@
       <c r="F31" t="s">
         <v>130</v>
       </c>
+      <c r="G31" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
@@ -1607,8 +1889,8 @@
       <c r="F32" t="s">
         <v>128</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>131</v>
+      <c r="G32" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1630,6 +1912,9 @@
       <c r="F33" t="s">
         <v>128</v>
       </c>
+      <c r="G33" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
@@ -1650,6 +1935,9 @@
       <c r="F34" t="s">
         <v>128</v>
       </c>
+      <c r="G34" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
@@ -1670,6 +1958,9 @@
       <c r="F35" t="s">
         <v>128</v>
       </c>
+      <c r="G35" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
@@ -1690,6 +1981,9 @@
       <c r="F36" t="s">
         <v>128</v>
       </c>
+      <c r="G36" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
@@ -1710,6 +2004,9 @@
       <c r="F37" t="s">
         <v>128</v>
       </c>
+      <c r="G37" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
@@ -1730,6 +2027,9 @@
       <c r="F38" t="s">
         <v>130</v>
       </c>
+      <c r="G38" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
@@ -1750,6 +2050,9 @@
       <c r="F39" t="s">
         <v>130</v>
       </c>
+      <c r="G39" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
@@ -1770,8 +2073,8 @@
       <c r="F40" t="s">
         <v>128</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>131</v>
+      <c r="G40" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1793,6 +2096,9 @@
       <c r="F41" t="s">
         <v>128</v>
       </c>
+      <c r="G41" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
@@ -1813,6 +2119,9 @@
       <c r="F42" t="s">
         <v>128</v>
       </c>
+      <c r="G42" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
@@ -1833,6 +2142,9 @@
       <c r="F43" t="s">
         <v>128</v>
       </c>
+      <c r="G43" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
@@ -1853,6 +2165,9 @@
       <c r="F44" t="s">
         <v>128</v>
       </c>
+      <c r="G44" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
@@ -1873,6 +2188,9 @@
       <c r="F45" t="s">
         <v>128</v>
       </c>
+      <c r="G45" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
@@ -1893,6 +2211,9 @@
       <c r="F46" t="s">
         <v>128</v>
       </c>
+      <c r="G46" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
@@ -1913,6 +2234,9 @@
       <c r="F47" t="s">
         <v>130</v>
       </c>
+      <c r="G47" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
@@ -1933,6 +2257,9 @@
       <c r="F48" t="s">
         <v>130</v>
       </c>
+      <c r="G48" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
@@ -1953,6 +2280,9 @@
       <c r="F49" t="s">
         <v>130</v>
       </c>
+      <c r="G49" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
@@ -1973,6 +2303,9 @@
       <c r="F50" t="s">
         <v>128</v>
       </c>
+      <c r="G50" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
@@ -1993,6 +2326,9 @@
       <c r="F51" t="s">
         <v>128</v>
       </c>
+      <c r="G51" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
@@ -2013,6 +2349,9 @@
       <c r="F52" t="s">
         <v>130</v>
       </c>
+      <c r="G52" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
@@ -2033,6 +2372,9 @@
       <c r="F53" t="s">
         <v>130</v>
       </c>
+      <c r="G53" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
@@ -2053,6 +2395,9 @@
       <c r="F54" t="s">
         <v>130</v>
       </c>
+      <c r="G54" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
@@ -2073,6 +2418,9 @@
       <c r="F55" t="s">
         <v>130</v>
       </c>
+      <c r="G55" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
@@ -2093,6 +2441,9 @@
       <c r="F56" t="s">
         <v>130</v>
       </c>
+      <c r="G56" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
@@ -2113,6 +2464,9 @@
       <c r="F57" t="s">
         <v>130</v>
       </c>
+      <c r="G57" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
@@ -2133,8 +2487,8 @@
       <c r="F58" t="s">
         <v>128</v>
       </c>
-      <c r="G58" s="4" t="s">
-        <v>131</v>
+      <c r="G58" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -2156,6 +2510,9 @@
       <c r="F59" t="s">
         <v>130</v>
       </c>
+      <c r="G59" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
@@ -2176,8 +2533,8 @@
       <c r="F60" t="s">
         <v>130</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>132</v>
+      <c r="G60" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -2199,6 +2556,9 @@
       <c r="F61" t="s">
         <v>129</v>
       </c>
+      <c r="G61" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
@@ -2219,8 +2579,8 @@
       <c r="F62" t="s">
         <v>129</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>133</v>
+      <c r="G62" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2242,6 +2602,9 @@
       <c r="F63" t="s">
         <v>129</v>
       </c>
+      <c r="G63" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
@@ -2262,19 +2625,22 @@
       <c r="F64" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G64" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E65">
         <v>125</v>
@@ -2282,19 +2648,22 @@
       <c r="F65" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G65" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E66">
         <v>56</v>
@@ -2302,8 +2671,11 @@
       <c r="F66" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G66" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>67</v>
       </c>
@@ -2322,8 +2694,11 @@
       <c r="F67" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G67" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>68</v>
       </c>
@@ -2342,8 +2717,11 @@
       <c r="F68" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G68" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>69</v>
       </c>
@@ -2362,8 +2740,11 @@
       <c r="F69" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G69" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>70</v>
       </c>
@@ -2382,8 +2763,11 @@
       <c r="F70" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G70" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>71</v>
       </c>
@@ -2402,8 +2786,11 @@
       <c r="F71" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G71" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B72" s="2" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
restored comments about suspicious nodules
</commit_message>
<xml_diff>
--- a/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
+++ b/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Github\bmen689_group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E723713C-BA96-44F6-BA97-431FC9A37AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AF108F-E230-4BDF-BCB9-7E41381997C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="-12540" windowWidth="14400" windowHeight="7365" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="209">
   <si>
     <t>LUNGx-CT001</t>
   </si>
@@ -649,13 +649,22 @@
   </si>
   <si>
     <t>LUNGx-CT060\02-20-2007-6367-CT INFUSED CHEST-13719\4-HIGH RES-42551\000035.dcm</t>
+  </si>
+  <si>
+    <t>looks like scarring</t>
+  </si>
+  <si>
+    <t>juxtapleural: are the center coordinates correct?</t>
+  </si>
+  <si>
+    <t>is this correct?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -671,13 +680,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -689,16 +710,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1129,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1145,7 +1169,7 @@
     <col min="6" max="6" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3">
         <v>1</v>
       </c>
@@ -1164,11 +1188,11 @@
       <c r="F1" t="s">
         <v>128</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -1187,20 +1211,20 @@
       <c r="F2" t="s">
         <v>128</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>136</v>
-      </c>
-      <c r="H2">
-        <v>24</v>
       </c>
       <c r="I2">
         <v>24</v>
       </c>
       <c r="J2">
+        <v>24</v>
+      </c>
+      <c r="K2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1219,14 +1243,14 @@
       <c r="F3" t="s">
         <v>128</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>137</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>43489</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1245,11 +1269,11 @@
       <c r="F4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1268,11 +1292,11 @@
       <c r="F5" t="s">
         <v>129</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1291,11 +1315,11 @@
       <c r="F6" t="s">
         <v>129</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1314,11 +1338,11 @@
       <c r="F7" t="s">
         <v>129</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -1337,11 +1361,11 @@
       <c r="F8" t="s">
         <v>128</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1360,11 +1384,11 @@
       <c r="F9" t="s">
         <v>129</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -1383,11 +1407,11 @@
       <c r="F10" t="s">
         <v>128</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -1406,11 +1430,11 @@
       <c r="F11" t="s">
         <v>128</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -1429,11 +1453,11 @@
       <c r="F12" t="s">
         <v>128</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -1452,11 +1476,11 @@
       <c r="F13" t="s">
         <v>128</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -1475,11 +1499,11 @@
       <c r="F14" t="s">
         <v>128</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -1498,11 +1522,11 @@
       <c r="F15" t="s">
         <v>129</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1521,11 +1545,11 @@
       <c r="F16" t="s">
         <v>128</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1544,11 +1568,11 @@
       <c r="F17" t="s">
         <v>129</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1567,11 +1591,11 @@
       <c r="F18" t="s">
         <v>129</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1590,11 +1614,11 @@
       <c r="F19" t="s">
         <v>129</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -1613,11 +1637,11 @@
       <c r="F20" t="s">
         <v>129</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1636,11 +1660,11 @@
       <c r="F21" t="s">
         <v>128</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1659,11 +1683,11 @@
       <c r="F22" t="s">
         <v>128</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1682,11 +1706,11 @@
       <c r="F23" t="s">
         <v>128</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1705,11 +1729,11 @@
       <c r="F24" t="s">
         <v>130</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1728,11 +1752,11 @@
       <c r="F25" t="s">
         <v>128</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>26</v>
       </c>
@@ -1751,11 +1775,11 @@
       <c r="F26" t="s">
         <v>130</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1774,11 +1798,11 @@
       <c r="F27" t="s">
         <v>130</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1797,11 +1821,11 @@
       <c r="F28" t="s">
         <v>128</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1820,11 +1844,11 @@
       <c r="F29" t="s">
         <v>128</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1843,11 +1867,11 @@
       <c r="F30" t="s">
         <v>130</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1866,11 +1890,11 @@
       <c r="F31" t="s">
         <v>130</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1889,11 +1913,14 @@
       <c r="F32" t="s">
         <v>128</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H32" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>33</v>
       </c>
@@ -1912,11 +1939,11 @@
       <c r="F33" t="s">
         <v>128</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>34</v>
       </c>
@@ -1935,11 +1962,11 @@
       <c r="F34" t="s">
         <v>128</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1958,11 +1985,11 @@
       <c r="F35" t="s">
         <v>128</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1981,11 +2008,11 @@
       <c r="F36" t="s">
         <v>128</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -2004,11 +2031,11 @@
       <c r="F37" t="s">
         <v>128</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -2027,11 +2054,11 @@
       <c r="F38" t="s">
         <v>130</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>39</v>
       </c>
@@ -2050,11 +2077,11 @@
       <c r="F39" t="s">
         <v>130</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>40</v>
       </c>
@@ -2073,11 +2100,14 @@
       <c r="F40" t="s">
         <v>128</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -2096,11 +2126,11 @@
       <c r="F41" t="s">
         <v>128</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -2119,11 +2149,11 @@
       <c r="F42" t="s">
         <v>128</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>43</v>
       </c>
@@ -2142,11 +2172,11 @@
       <c r="F43" t="s">
         <v>128</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>44</v>
       </c>
@@ -2165,11 +2195,11 @@
       <c r="F44" t="s">
         <v>128</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -2188,11 +2218,11 @@
       <c r="F45" t="s">
         <v>128</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -2211,11 +2241,11 @@
       <c r="F46" t="s">
         <v>128</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>47</v>
       </c>
@@ -2234,11 +2264,11 @@
       <c r="F47" t="s">
         <v>130</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -2257,11 +2287,11 @@
       <c r="F48" t="s">
         <v>130</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>49</v>
       </c>
@@ -2280,11 +2310,11 @@
       <c r="F49" t="s">
         <v>130</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>50</v>
       </c>
@@ -2303,11 +2333,11 @@
       <c r="F50" t="s">
         <v>128</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -2326,11 +2356,11 @@
       <c r="F51" t="s">
         <v>128</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -2349,11 +2379,11 @@
       <c r="F52" t="s">
         <v>130</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -2372,11 +2402,11 @@
       <c r="F53" t="s">
         <v>130</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -2395,11 +2425,11 @@
       <c r="F54" t="s">
         <v>130</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -2418,11 +2448,11 @@
       <c r="F55" t="s">
         <v>130</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>56</v>
       </c>
@@ -2441,11 +2471,11 @@
       <c r="F56" t="s">
         <v>130</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -2464,11 +2494,11 @@
       <c r="F57" t="s">
         <v>130</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>58</v>
       </c>
@@ -2487,11 +2517,14 @@
       <c r="F58" t="s">
         <v>128</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H58" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>59</v>
       </c>
@@ -2510,11 +2543,11 @@
       <c r="F59" t="s">
         <v>130</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>60</v>
       </c>
@@ -2533,11 +2566,14 @@
       <c r="F60" t="s">
         <v>130</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H60" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>61</v>
       </c>
@@ -2556,11 +2592,11 @@
       <c r="F61" t="s">
         <v>129</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -2579,11 +2615,14 @@
       <c r="F62" t="s">
         <v>129</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H62" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>63</v>
       </c>
@@ -2602,11 +2641,11 @@
       <c r="F63" t="s">
         <v>129</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>64</v>
       </c>
@@ -2625,11 +2664,11 @@
       <c r="F64" t="s">
         <v>129</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -2648,11 +2687,11 @@
       <c r="F65" t="s">
         <v>129</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>66</v>
       </c>
@@ -2671,11 +2710,11 @@
       <c r="F66" t="s">
         <v>129</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>67</v>
       </c>
@@ -2694,11 +2733,11 @@
       <c r="F67" t="s">
         <v>128</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>68</v>
       </c>
@@ -2717,11 +2756,11 @@
       <c r="F68" t="s">
         <v>128</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>69</v>
       </c>
@@ -2740,11 +2779,11 @@
       <c r="F69" t="s">
         <v>128</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>70</v>
       </c>
@@ -2763,11 +2802,11 @@
       <c r="F70" t="s">
         <v>128</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>71</v>
       </c>
@@ -2786,11 +2825,11 @@
       <c r="F71" t="s">
         <v>128</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B72" s="2" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
- adding list of features to be removed to generate clean dataset - ROC code generator - script to generate CSV training file from images - anotations of ground truth
</commit_message>
<xml_diff>
--- a/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
+++ b/TestSet_NoduleData_PublicRelease_wTruth (exclude suspicious).xlsx
@@ -5,17 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Github\bmen689_group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmjch\Dropbox\PhD\Courses\2019 - C - Fall\BMEN689 - ML and CV in BMEN\Project\prog\github\bmen689_group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2325A27E-33A1-435C-8272-A048B75C263A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C6683A-F856-42C9-A40A-2D42E4B8A91D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5272" yWindow="2228" windowWidth="15248" windowHeight="10852" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="141">
   <si>
     <t>LUNGx-CT001</t>
   </si>
@@ -445,6 +445,15 @@
   </si>
   <si>
     <t>209, 308</t>
+  </si>
+  <si>
+    <t>Very noisy</t>
+  </si>
+  <si>
+    <t>kinda noisy</t>
+  </si>
+  <si>
+    <t>very noisy</t>
   </si>
 </sst>
 </file>
@@ -942,21 +951,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.08203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.0625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.1875" customWidth="1"/>
+    <col min="3" max="3" width="8.1875" customWidth="1"/>
+    <col min="4" max="4" width="14.1875" customWidth="1"/>
+    <col min="5" max="5" width="12.8125" customWidth="1"/>
+    <col min="6" max="6" width="26.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" s="3">
         <v>1</v>
       </c>
@@ -975,8 +984,11 @@
       <c r="F1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -1005,7 +1017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1028,7 +1040,7 @@
         <v>43489</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1068,7 +1080,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1088,7 +1100,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1107,8 +1119,11 @@
       <c r="F7" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -1128,7 +1143,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1148,7 +1163,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -1167,8 +1182,11 @@
       <c r="F10" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -1188,7 +1206,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -1208,7 +1226,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -1228,7 +1246,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -1247,8 +1265,11 @@
       <c r="F14" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -1267,8 +1288,11 @@
       <c r="F15" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1287,8 +1311,11 @@
       <c r="F16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1308,7 +1335,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1328,7 +1355,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1348,7 +1375,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -1367,8 +1394,11 @@
       <c r="F20" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1387,8 +1417,11 @@
       <c r="F21" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1408,7 +1441,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1428,7 +1461,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1448,7 +1481,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1467,8 +1500,11 @@
       <c r="F25" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" s="3">
         <v>26</v>
       </c>
@@ -1487,8 +1523,11 @@
       <c r="F26" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1508,7 +1547,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1528,7 +1567,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1547,8 +1586,11 @@
       <c r="F29" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1568,7 +1610,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1587,8 +1629,11 @@
       <c r="F31" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1611,7 +1656,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33" s="3">
         <v>33</v>
       </c>
@@ -1631,7 +1676,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A34" s="3">
         <v>34</v>
       </c>
@@ -1650,8 +1695,11 @@
       <c r="F34" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1670,8 +1718,11 @@
       <c r="F35" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1691,7 +1742,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1711,7 +1762,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1730,8 +1781,11 @@
       <c r="F38" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39" s="3">
         <v>39</v>
       </c>
@@ -1751,7 +1805,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A40" s="3">
         <v>40</v>
       </c>
@@ -1773,8 +1827,11 @@
       <c r="G40" s="4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -1794,7 +1851,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -1814,7 +1871,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A43" s="3">
         <v>43</v>
       </c>
@@ -1834,7 +1891,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A44" s="3">
         <v>44</v>
       </c>
@@ -1854,7 +1911,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -1874,7 +1931,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -1894,7 +1951,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A47" s="3">
         <v>47</v>
       </c>
@@ -1914,7 +1971,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -1934,7 +1991,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A49" s="3">
         <v>49</v>
       </c>
@@ -1953,8 +2010,11 @@
       <c r="F49" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A50" s="3">
         <v>50</v>
       </c>
@@ -1974,7 +2034,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -1994,7 +2054,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -2014,7 +2074,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -2034,7 +2094,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -2054,7 +2114,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -2074,7 +2134,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A56" s="3">
         <v>56</v>
       </c>
@@ -2094,7 +2154,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -2114,7 +2174,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A58" s="3">
         <v>58</v>
       </c>
@@ -2136,8 +2196,11 @@
       <c r="G58" s="4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H58" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A59" s="3">
         <v>59</v>
       </c>
@@ -2157,7 +2220,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A60" s="3">
         <v>60</v>
       </c>
@@ -2180,7 +2243,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A61" s="3">
         <v>61</v>
       </c>
@@ -2200,7 +2263,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -2222,8 +2285,11 @@
       <c r="G62" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A63" s="3">
         <v>63</v>
       </c>
@@ -2243,7 +2309,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A64" s="3">
         <v>64</v>
       </c>
@@ -2263,7 +2329,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -2283,7 +2349,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A66" s="3">
         <v>66</v>
       </c>
@@ -2303,7 +2369,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A67" s="3">
         <v>67</v>
       </c>
@@ -2323,7 +2389,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A68" s="3">
         <v>68</v>
       </c>
@@ -2342,8 +2408,11 @@
       <c r="F68" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G68" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A69" s="3">
         <v>69</v>
       </c>
@@ -2362,8 +2431,11 @@
       <c r="F69" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G69" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A70" s="3">
         <v>70</v>
       </c>
@@ -2383,7 +2455,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A71" s="3">
         <v>71</v>
       </c>
@@ -2403,7 +2475,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B72" s="2" t="s">
         <v>127</v>
       </c>

</xml_diff>